<commit_message>
add phonemes to responses, latest data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaiusz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaiusz\Desktop\asd\dtu\RAI\ECS-experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C4AD4F-68FA-47C0-AF77-C5A8EB6B9FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B6415-C74F-468A-B508-35D25E34D378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="106">
+  <si>
+    <t>Participant ID</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
   <si>
     <t>muBD79cjOL5</t>
   </si>
@@ -196,6 +205,12 @@
     <t>[{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"}]</t>
   </si>
   <si>
+    <t>QDFm6GGoXRn</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"}]</t>
+  </si>
+  <si>
     <t>vdHAiEwzZ3i</t>
   </si>
   <si>
@@ -295,13 +310,34 @@
     <t>[{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"}]</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>response</t>
+    <t>LBrgmOtfoeS</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"}]</t>
+  </si>
+  <si>
+    <t>mkGml8GhHRC</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"}]</t>
+  </si>
+  <si>
+    <t>iPyJuhNskr7</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"}]</t>
+  </si>
+  <si>
+    <t>r2KtT8v1BrH</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"}]</t>
+  </si>
+  <si>
+    <t>oTd7YEISp3l</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"}]</t>
   </si>
 </sst>
 </file>
@@ -563,518 +599,576 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
phoneme pair update and latest data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaiusz\Desktop\asd\dtu\RAI\ECS-experiment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B6415-C74F-468A-B508-35D25E34D378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="130">
   <si>
     <t>Participant ID</t>
   </si>
@@ -211,6 +202,42 @@
     <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"}]</t>
   </si>
   <si>
+    <t>P3SEIZnX6k3</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"}]</t>
+  </si>
+  <si>
+    <t>rXaJ2sWSnuk</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"}]</t>
+  </si>
+  <si>
+    <t>GSiXF9sB7Lu</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"}]</t>
+  </si>
+  <si>
+    <t>X3YZI52B3Qe</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"}]</t>
+  </si>
+  <si>
+    <t>ndIPuTc6WNs</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"}]</t>
+  </si>
+  <si>
+    <t>UpHbfcJxkeJ</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"}]</t>
+  </si>
+  <si>
     <t>vdHAiEwzZ3i</t>
   </si>
   <si>
@@ -338,21 +365,56 @@
   </si>
   <si>
     <t>[{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"}]</t>
+  </si>
+  <si>
+    <t>XcVhPNabrOL</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"}]</t>
+  </si>
+  <si>
+    <t>XWLqjVHufIJ</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"mølle","word2":"mulle"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"lys","word2":"lys"}]</t>
+  </si>
+  <si>
+    <t>2SjTHoDevt6</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"}]</t>
+  </si>
+  <si>
+    <t>zchpgnvwRAe</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"røre","word2":"røre"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"pil","word2":"bil"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"}]</t>
+  </si>
+  <si>
+    <t>qCpN9NJtOIx</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"fuld","word2":"fugl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"møl","word2":"møl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"tat","word2":"tæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ful","word2":"ful"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lidt","word2":"let"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"set","word2":"sæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"syr","word2":"syr"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"syn","word2":"søn"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"gul","word2":"guld"}]</t>
+  </si>
+  <si>
+    <t>645a1Zg2j0U</t>
+  </si>
+  <si>
+    <t>[{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"ven","word2":"pen"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rør","word2":"rær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"mæt","word2":"mæt"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"set","word2":"sæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"mølle","word2":"mulle"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"ful","word2":"ful"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"ful","word2":"fyl"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"lys","word2":"los"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"ben","word2":"bøn"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"lød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fisk","word2":"fæsk"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"kat","word2":"kat"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"røre","word2":"røre"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"lys","word2":"lys"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"tat","word2":"tæt"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"sø","word2":"su"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"løg","word2":"ly"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"dør","word2":"dør"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"fuld","word2":"fuld"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"pil","word2":"bil"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"rød","word2":"ryd"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syn","word2":"søn"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"fuld","word2":"fugl"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"kat","word2":"kæt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"møl","word2":"møl"},{"participantResponse":"different","correctResponse":"same","isCorrect":false,"word1":"nø","word2":"nø"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"sinde","word2":"sende"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"væg","word2":"vægt"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"skæl","word2":"skæl"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"ben","word2":"ben"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"lidt","word2":"let"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"grå","word2":"grå"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"gul","word2":"guld"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"rød","word2":"rød"},{"participantResponse":"same","correctResponse":"different","isCorrect":false,"word1":"syd","word2":"sød"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"før","word2":"fær"},{"participantResponse":"same","correctResponse":"same","isCorrect":true,"word1":"syr","word2":"syr"},{"participantResponse":"different","correctResponse":"different","isCorrect":true,"word1":"nø","word2":"nu"}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -363,43 +425,36 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -589,25 +644,20 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +670,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -631,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,7 +692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -653,7 +703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -664,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -675,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -686,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -697,7 +747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -708,7 +758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -719,7 +769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -730,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -741,7 +791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -752,7 +802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -763,7 +813,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -774,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -785,7 +835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -796,7 +846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -807,7 +857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -818,7 +868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -829,7 +879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -840,7 +890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -851,7 +901,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -862,7 +912,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -873,7 +923,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -884,7 +934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -895,7 +945,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -906,7 +956,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -917,7 +967,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -928,7 +978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
@@ -939,238 +989,370 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="1" t="s">
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1" t="s">
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1" t="s">
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="1" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="1" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>